<commit_message>
finished first version of plotting system
</commit_message>
<xml_diff>
--- a/data/varioscan_layout.xlsx
+++ b/data/varioscan_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michiel/git_projects/Rprojects/growthis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D32A839-A142-B349-88E0-4FFB87389366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0573804-CCC4-EC45-B492-80238E54FCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{C323172E-B3B3-FC42-83F7-37D2828FD84F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>bacterie:</t>
-  </si>
-  <si>
-    <t>E.coli</t>
   </si>
   <si>
     <t>zonder bacterie</t>
@@ -243,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -295,9 +289,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,17 +625,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EBB5D2-636C-BD4A-A00F-104D11206F67}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -727,7 +718,7 @@
       <c r="M4" s="10">
         <v>0.02</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="28">
         <v>0.02</v>
       </c>
     </row>
@@ -768,7 +759,7 @@
       <c r="M5" s="10">
         <v>0.01</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5" s="28">
         <v>0.01</v>
       </c>
     </row>
@@ -809,7 +800,7 @@
       <c r="M6" s="15">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -850,7 +841,7 @@
       <c r="M7" s="15">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="29">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
@@ -891,7 +882,7 @@
       <c r="M8" s="15">
         <v>1.25E-3</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="29">
         <v>1.25E-3</v>
       </c>
     </row>
@@ -932,7 +923,7 @@
       <c r="M9" s="15">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="N9" s="30">
+      <c r="N9" s="29">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
@@ -973,7 +964,7 @@
       <c r="M10" s="15">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="29">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
@@ -1002,7 +993,7 @@
       <c r="I11" s="17">
         <v>0</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="27">
         <v>0</v>
       </c>
       <c r="K11" s="17">
@@ -1022,77 +1013,69 @@
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="22"/>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="21" t="s">
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="24"/>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="23"/>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="27"/>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
+      <c r="B21" s="26"/>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>